<commit_message>
[DOCS] Main documentation & report WIP
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/ColdPlasma_Data_1.xlsx
+++ b/Documentation/Experiments/ColdPlasma_Data_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PICADOR-Jr-2025\Documentation\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96018033-6E24-4B60-AEBB-2CFD32ACF2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D73765-6D86-409F-9F63-51E1CF7B75B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="240" windowWidth="38640" windowHeight="20505" activeTab="1" xr2:uid="{36E27A8F-5961-4EE6-92B3-CCF1250CFAD0}"/>
+    <workbookView xWindow="6465" yWindow="240" windowWidth="38640" windowHeight="20505" xr2:uid="{36E27A8F-5961-4EE6-92B3-CCF1250CFAD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="1" r:id="rId1"/>
@@ -6326,7 +6326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC169F66-A126-4993-8114-DCD71261FFA1}">
   <dimension ref="A1:B3019"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -30436,7 +30436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BB9A94-993F-4ABE-8543-C750D2B48CC9}">
   <dimension ref="A1:C611"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>

</xml_diff>